<commit_message>
New links to bibliography and new i button font
</commit_message>
<xml_diff>
--- a/content/EcoHealthContent.xlsx
+++ b/content/EcoHealthContent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\PRIV\NERL_LEB\Other Projects\A-M\KumarSudha\EcoHealthBrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC9E8F7-A0F4-4A4D-898D-65CBD3D3C09C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32903665-A583-4E0B-A098-751A291AFACA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="28785" windowHeight="15450" tabRatio="688" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8865" yWindow="315" windowWidth="15885" windowHeight="17370" tabRatio="688" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ecosystems" sheetId="1" r:id="rId1"/>
@@ -7882,9 +7882,6 @@
 &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Marselle_2013” target=”_blank”&gt;Marselle et al., 2013; n=708, England&lt;/a&gt;). [7] Those who engaged in physical activity while immersed in natural settings had a more positive affect when compared with sedentary individuals and those physically active in a laboratory setting (p less than 0.01) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kinnafick_2014” target=”_blank”&gt;Kinnafick and Thogersen-Ntoumani, 2014; n=40, United Kingdom&lt;/a&gt;). [8] Walking in a natural environment with a limited field of vision and with opportunities for concealment significantly increased reported levels of sadness relative to pre-walk status (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Gatersleben_2013” target=”_blank”&gt;Gatersleben et al., 2013; n=17, southern England&lt;/a&gt;). [9] Also, biodiversity might be associated with happiness, as individuals that visited parks with greater plant diversity levels reported higher levels of happiness (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Adinolfi_2014” target=”_blank”&gt;Suarez et al., 2014; 2014; n=10, Grenada, Spain&lt;/a&gt;). [10] Study participants who were shown various photos of urban or natural settings following the viewing of a stressful video reported improved positive feelings after viewing the natural settings (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Ulrich_1991” target=”_blank”&gt;Ulrich 1991; n=120, Delaware&lt;/a&gt;). [11] In a study comparing two neighborhoods with varying levels of green space, those in the greener neighborhood reported higher levels of satisfaction and happiness (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Van_2011” target=”_blank”&gt;Herzele and de Vries 2011; n=190, Belgium&lt;/a&gt;). [12] As engagement with natural beauty increased by one unit, life satisfaction was predicted to increase by 15% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZhangJW_2014” target=”_blank”&gt;Zhang et al., 2014; n=Study 1: 1108, Study 2: 151; Berkeley, CA&lt;/a&gt;). </t>
   </si>
   <si>
-    <t xml:space="preserve">Various ecologically-based filtration systems, constructed in locations where urban stormwater runs or accumulates, have been shown to reduce contaminants in water by 29 to 99% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Birch_2005” target=”_blank”&gt;Birch et al., 2005; DiBlasi et al., 2008&lt;/a&gt;). These systems can include stormwater infiltration basins, grass swales, rain gardens, and stormwater bioretention facilities. The systems were able to remove 69% of suspended solids, 46% of phosphorous (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Deletic_2006” target=”_blank”&gt;Deletic and Fletcher, 2006&lt;/a&gt;), 51-56% of nitrogen (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dietz_2005” target=”_blank”&gt;Dietz and Clausen, 2005; Deletic and Fletcher, 2006&lt;/a&gt;), 90% of polycyclic aromatic hydrocarbons (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#DiBlasi_2008” target=”_blank”&gt;DiBlasi et al., 2008&lt;/a&gt;), and 29-93% of heavy metals (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Birch_2005” target=”_blank”&gt;Birch et al., 2005&lt;/a&gt;). A large nursery-based study evaluated the effectiveness of 9 native plants in their nutrient (PO4-3, NH3, NO3-) removal capacity from urban stormwater. Six of the best performers (Agapanthus, Pennisetum, Stenotaphrum, Zantedeschia, Phragmites and Typha) removed 16% more PO4-3 compared to soil-only control; two plant types (Pennisetum and Stenotaphrum) were 22% more effective in removing NH3 compared to control, and five (Agapanthus, Carpobrotus, Ficinia, Zantedeschia and Typha) removed 27-53% more NO3- compared to their controls (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Milandri_2012” target=”_blank”&gt;Milandri et al., 2012&lt;/a&gt;). </t>
-  </si>
-  <si>
     <t>Missing Id: Deutsch et al., 2005, Mentens et al., 2005</t>
   </si>
   <si>
@@ -7894,10 +7891,6 @@
     <t>Missing Id:  Fan et al., 2015, Jeppesen et al., 2014</t>
   </si>
   <si>
-    <t xml:space="preserve">*Access or proximity to green space*  Many studies have found that people who live close to green space visit them more frequently and thus increase their time spent in physical activity, both at the green space itself and walking or biking to the area instead of driving (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Giles_2005” target=”_blank”&gt;Giles-Corti et al., 2005&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mowen_2007” target=”_blank”&gt;Mowen et al., 2007; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grigsby_2011” target=”_blank”&gt;Grigsby-Toussaint et al., 2011&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wendel_2004” target=”_blank”&gt;Wendel-Vos et al., 2004&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenDA_2006” target=”_blank”&gt;Cohen et al., 2006&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Edwards_2014” target=”_blank”&gt;Edwards et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#HanB_2014” target=”_blank”&gt;Han et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lachowycz_2014” target=”_blank”&gt;Lachowycz and Jones, 2014&lt;/a&gt;). One study found that living in an area with high parkland density (greater than 0.14%) increased the odds (OR=1.19) of meeting federal guidelines for MVPA and VPA (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#West_2012” target=”_blank”&gt;West et al., 2012&lt;/a&gt;). Another study found that as the density of public green space increased by one unit, walking was predicted to increase by 8.6% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Pliakas_2014” target=”_blank”&gt;Pliakas et al., 201&lt;/a4&gt;). A Swedish study found that people with green spaces within 50m of their homes visited those spaces 4x as much as those whose closest green space was 1km away (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grahn_2003” target=”_blank”&gt;Grahn and Stigsdotter, 2003&lt;/a&gt;). In San Diego, the presence of a park within a 50-meter buffer of each accelerometer study point was associated with 41% higher odds (OR 1.41) of light physical activity in adolescent females (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rodriguez_2012” target=”_blank”&gt;Rodriguez et al., 2012; n=293&lt;/a&gt;). However, several studies have found little to no association between access or proximity to green space and physical activity (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Hillsdon_2006” target=”_blank”&gt;Hillsdon et al., 2006&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Maas_2008” target=”_blank”&gt;Maas et al., 2008&lt;/a&gt;). *Amount and design of green space:* The size of nearby public open spaces has been positively associated with physical activity (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Paquet_2013” target=”_blank”&gt;Paquet et al., 2013&lt;/a&gt;; Fan et al., 2015&lt;/a&gt;). Positive correlations have been found between number of park visitors, as well as diversity of visitor activities, and number of trees and canopy coverage (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Adinolfi_2014” target=”_blank”&gt;Adinolfi et al., 2014&lt;/a&gt;). One study found that individuals living in the greenest urban quintile were 1.39 times more physically active than those living in the least green urban quintile (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mytton_2012” target=”_blank”&gt;Mytton et al., 2012&lt;/a&gt;). Another study reported that respondents whose residential environment contained high levels of greenery (on a scale from 1-5) were 3x more likely to be physically active, and 40% less likely to be overweight or obese (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Ellaway_2005” target=”_blank”&gt;Ellaway et al., 2005&lt;/a&gt;). Yet another study found that increased exposure to neighborhood greenness from 10th to 90th percentile was associated with a 34% to 39% increase in odds for moderate to vigorous physical activity (MVPA) in children (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Almanza_2012” target=”_blank”&gt;Almanza et al., 2012&lt;/a&gt;). Cross-sectional study of middle-school aged children found that a 5% increase in neighborhood area covered by trees was associated with 5% higher frequency of physical activity outside of school hours (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#JanssenI_2015” target=”_blank”&gt;Janssen and Rosu, 2015&lt;/a&gt;). Elderly men were shown to participate in regular physical activity when living within a 400-meter radius green space buffer around the home (OR=1.21) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Gong_2014” target=”_blank”&gt;Gong et al., 2014&lt;/a&gt;). Strong positive associations were reported between the odds of walking and both density of street trees and street network connectivity, and also between distance walked and both overall greenness and density of street trees (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Sarkar_2015” target=”_blank”&gt;Sarkar et al., 2015&lt;/a&gt;). &amp;#xD;&amp;#xD;In urban areas, street intersections and other pedestrian amenities are a promoting factor in physical activity (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wetter_2001” target=”_blank”&gt;Wetter et al., 2001&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kaczynski_2014” target=”_blank”&gt;Kaczynski et al., 2014&lt;/a&gt;). Children engaged in significantly greater amounts of MVPA and PA after the conversion of a traditional playground or school yard into one modeled on natural environments (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Coe_2014” target=”_blank”&gt;Coe et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#JanssonM_2014” target=”_blank”&gt;Jansson et al., 2014&lt;/a&gt;), or when community spaces were comprised of vegetation, open meadows, and/or undulating topography (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lestan_2014” target=”_blank”&gt;Lestan et al., 2014&lt;/a&gt;). However, while school areas with the greatest amount of green space were among children&amp;#39;s favorites, the areas of mixed green and built environments were where the most physical activity took place (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Martensson_2014” target=”_blank”&gt;Martensson et al., 2014&lt;/a&gt;). *Perceptions of green space* Increases in individual satisfaction with neighborhood green space, perception of recreation areas, and perception of their easy access were found to be contributing factors to increases in overall MVPA and PA in parks (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Bai_2013” target=”_blank”&gt;
-Bai et al., 2013&lt;/a&gt;; Jeppesen et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jongeneel_2014” target=”_blank”&gt;Jongeneel-Grimen et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#LeeJ_2014” target=”_blank”&gt;Lee et al., 2014&lt;/a&gt;). A multi-country study found that adult recreational walking was strongly associated with perceived neighborhood environmental attributes such as land use mix, street connectivity and aesthetics (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Sugiyama_2014” target=”_blank”&gt;Sugiyama et al., 2014&lt;/a&gt;). One study found that, in a living environment perceived as green, 62% of the aging population engaged in high levels of physical activity while only 11% engaged in physical activity in an environment perceived as containing little green space (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kemperman_2014” target=”_blank”&gt;Kemperman and Timmermans, 2014&lt;/a&gt;). Also, being nature-oriented was more important than park access as a predictor of park use (p less than 0.01) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lin_2014” target=”_blank”&gt;Lin et al., 2014&lt;/a&gt;). &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZhangW_2015” target=”_blank”&gt;Zhang et al. (2015)&lt;/a&gt; found that five variables had significant effects on respondents&amp;#39; satisfaction levels when participating in physical activities in urban green spaces: housing price of the residential units where respondents lived (p=0.001), travel time to the nearest park (p less than 0.0001), counts of types of green spaces available for physical activities (p=0.04), and the rating of vegetation (p less than 0.0001). </t>
-  </si>
-  <si>
     <t xml:space="preserve">A study in a mixed agricultural landscape examined water infiltration rates through course- and fine-textured soils within four vegetation types: native Eucalypt and Cypress trees, intertree perennial grasses, and cultivated zones with annual crops. On fine-textured soils, steady-state infiltration rates were almost five-fold greater under Eucalypt and Cypress tree canopies than under grassed or cultivated landscapes. These differences were attributed to greater proportion of macropores (large soil pores) under trees than other vegetation types. (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Eldridge_2005” target=”_blank”&gt;Eldridge and Freudenberger, 2005&lt;/a&gt;). </t>
   </si>
   <si>
@@ -7949,19 +7942,10 @@
     <t xml:space="preserve">Conifer species have the highest minimum and maximum surface water storage capacities. The mean storage capacities were nearly 2 times greater for coniferous species than for broadleaf evergreen and broadleaf deciduous species (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#XiaoQ_2016” target=”_blank”&gt;Xiao and McPherson, 2015&lt;/a&gt;). Among desert shrubs, mean canopy water storage capacity (expressed in water storage per leaf area) was greater for needled shrubs (A. ordosica=0.61 mm) than for ovate-leaved shrubs (C. korshinskii=0.39 mm and H. scoparium=0.43 mm) when rainfall intensities ranged from 1.15 to 11.53 mm h-1 (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#WangXP_2012” target=”_blank”&gt;Wang et al., 2012&lt;/a&gt;). In semi-arid landscapes including dry grasslands and thorn shrublands, greater plant cover can reduce precipitation-generated runoff compared to bare soil plots (Greene_1994Greene et al., 1994&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Chirino_2006” target=”_blank”&gt;Chirino et al., 2006&lt;/a&gt;). Infiltration rates and resistance to overland flow were found to be approximately 10 and 4 times greater, respectively, on grassland compared to shrubland hillslopes (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Abrahams_1994” target=”_blank”&gt;Abrahams et al., 1994&lt;/a&gt;). Another study revealed that grassland communities generated 150% less runoff under simulated rainfall conditions than shrubland communities (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Neave_2002” target=”_blank”&gt;Neave and Abrahams, 2002&lt;/a&gt;). Green roofs in dryland urban environments can reduce the impacts of stormwater runoff as well; rooftops consisting of succulent, shrub, and herbaceous plant species reduced water runoff by more than 80-90% compared to bare rooftops (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nardini_2012” target=”_blank”&gt;Nardini et al., 2012&lt;/a&gt;; Volder and Dvorak, 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Biological soil crusts can also reduce runoff and increase infiltration rates and water storage capacity. One study reported a 27% reduction in rainfall runoff by artificially propagated soil crusts after the first three years of inoculation compared to control plots (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#XiaoQ_2016” target=”_blank”&gt;Xiao et al., 2015&lt;/a&gt;). Runoff volume was found to be two times greater on cyanobacterial crusts than on lichen crusts (H=14.63, p=0.0001) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lazaro_2014” target=”_blank”&gt;Lazaro and Mora, 2014&lt;/a&gt;). Runoff from biocrust patches was found to be 2.6 times greater than that from shrub patches (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#LiXJ_2008” target=”_blank”&gt;Li et al., 2008&lt;/a&gt;). Infiltration rates were 3.4-times greater through the biological soil crust than through rabbit-disturbed soils (F1.16=47.8, p less than 0.001) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Eldridge_2010” target=”_blank”&gt;Eldridge et al., 2010&lt;/a&gt;). Artificial destruction of moss-dominated biological soil crusts decreased soil water content by up to 18% and decreased water storage in the soil (first 0-90cm) by 7.8mm, 4.4mm, 8.0mm, and 4.9mm in the second, third, fourth, and seventh year, respectively (Xiao et al., 2014). </t>
   </si>
   <si>
-    <t xml:space="preserve">Vegetative cover in urban and rural desert environments can reduce ambient air pollutant concentrations both by removal and by airflow displacement. Pinyon-juniper stands have shown the highest capacity to remove criteria air pollutants (e.g., PM10, O3, NO2), followed by shrublands and grasslands (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dicus_2009” target=”_blank”&gt;Dicus et al., 2009&lt;/a&gt;). Mean ambient NOx and PM10 have been measured at 89ppb and 24 mg/m3, respectively, in urban parks, while means for an urban street were 413ppb and 80 mg/m3, respectively (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenP_2014” target=”_blank”&gt;Cohen et al., 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Dust storms are frequent in dryland environments, where low-pressure and high wind-speed conditions can increase average PM2.5 and PM10 concentrations (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZangR_2008” target=”_blank”&gt;Zhang et al., 2008&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Hosseini_2015” target=”_blank”&gt;Hosseini et al., 2015&lt;/a&gt;). Naturally-occurring biological soil crusts (biocrusts) and vegetative cover (e.g., trees, shrubs, grasses) can decrease soil erosion rates by holding soil in place and/or by reducing wind. For example, during periods of dust flow, park trees were found to reduce PM10 from 218 micro-g/m3 to 64 micro-g/m3 (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenP_2014” target=”_blank”&gt;Cohen et al., 2014&lt;/a&gt;). Significant negative correlation (-0.59 at 99% CI) have been observed between vegetative cover and occurrences of spring dust storms (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Zou_2004” target=”_blank”&gt;Zou and Zhai 2004&lt;/a&gt;). Experimental plots with 100% grass cover reductions experienced 10 times greater erosion rates than control plots with 0% grass cover reductions (p=0.05) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#LiJ_2007” target=”_blank”&gt;Li et al., 2007&lt;/a&gt;). Furrowing and seeding three native perennial shrubs and bunch grass in previously tilled or over-grazed land helped reduce fugitive dust emissions by more than 80% by adequately stabilizing soil (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grants_1998” target=”_blank”&gt;Grantz et al., 1998). At wind velocities of 18, 22, and 25 m/s, soil covered with 90% biocrust had wind erosion rates (g/min) 46, 21, and 17 times lower than those on sandy soil with 0% biocrust (Zhang et al., 2006). </t>
-  </si>
-  <si>
     <t>Zhang YM, HL Wang, et al. 2006 has Id as "ZhangX_2010" is that right? , Is it Grants or Grantz?</t>
   </si>
   <si>
     <t xml:space="preserve">Forested stream buffers have been found to remove up to 100% of nitrogen (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Schoonover_2005” target=”_blank”&gt;Schoonover et al., 2005&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Vidon_2004” target=”_blank”&gt;Vidon and Hill 2004&lt;/a&gt;), 89% of phosphorous (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Syversen_2005” target=”_blank”&gt;Syversen et al., 2005&lt;/a&gt;), 91% of particles (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Syversen_2005” target=”_blank”&gt;Syversen et al., 2005&lt;/a&gt;), 97% of sediment (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#LeeKH_2003” target=”_blank”&gt;Lee et al., 2003&lt;/a&gt;), and 100% of certain pesticides (Schulz and Peall 2000&lt;/a&gt;) that were measured in surface runoff. Studies have shown that within forested stream buffers, nitrogen and pesticide removal efficiency increase exponentially with buffer width (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZhangX_2010” target=”_blank”&gt;Zhang et al., 2010&lt;/a&gt;) and that trees are more efficient at removal than grasses alone or trees and grasses combined (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZhangX_2010” target=”_blank”&gt;Zhang et al., 2010&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Hefting_2005” target=”_blank”&gt;Hefting et al., 2005&lt;/a&gt;). In rural Africa, the presence of forest cover within 25 km&amp;#178; of the home has been linked to decreased odds of diarrhea in children less than 5 years old: from 15% (at 10-19% forest cover) to 92% (at 50-59% forest cover); these findings suggest natural filtration of drinking water sources (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Johnson_2013” target=”_blank”&gt;Johnson et al., 2013&lt;/a&gt;). For high-intensity land use, a 60-meter forested stream buffer is recommended, for moderate, 45 meters, and low, 30 meters. To protect isolated water bodies and wetlands, a 120m buffer is recommended and for steep slopes and/or cleared hills a 40m buffer is recommended (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Hansen_2010” target=”_blank”&gt;Hansen et al., 2010&lt;/a&gt;). </t>
-  </si>
-  <si>
-    <t>Urban tree cover and other green space can reduce local concentrations of harmful air pollutants. *Mitigation of PM10*  Multiple modeling studies have linked tree cover to a 1-2% local reduction in particulate matter smaller than 10 micrometers (PM10). Annually, this can equate to more than 100 metric tons in Mexico City (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Baumgardner_2012” target=”_blank”&gt;Baumgardner et al., 2012&lt;/a&gt;) and more than 2,000 metric tons in the city of London (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Tallis_2011” target=”_blank”&gt;Tallis et al., 2011&lt;/a&gt;). With strategic tree placement, annual reductions in ambient concentrations of PM10 may reach 7-20% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Bealey_2006” target=”_blank”&gt;Bealey et al., 2006&lt;/a&gt;). Hedge shrubbery has been found to collect PM10 with 34% efficiency (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Tiwary_2008” target=”_blank”&gt;Tiwary et al., 2008&lt;/a&gt;). Conifers and broad-leaved species with rough surfaces, and species with high leaf wax capture the highest quantities of PM (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Beckett_2000” target=”_blank”&gt;Beckett et al., 2000&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Popek_2013” target=”_blank”&gt;Popek et al., 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rasanen_2013” target=”_blank”&gt;Rasanen et al., 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nguyen_2015” target=”_blank”&gt;Nguyen et al., 2015&lt;/a&gt;). *Urban tree cover and mitigation of additional air pollutants*  In addition to PM10, trees can reduce ambient concentrations of PM2.5, ultrafine particles (less than 1 micrometer) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Beckett_2000” target=”_blank”&gt;Beckett et al., 2000&lt;/a&gt;) and gaseous pollutants including ozone, nitrogen dioxide, sulfur dioxide, and carbon monoxide (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nowak_1994” target=”_blank”&gt;Nowak et al., 1994&lt;/a&gt;). Based on an air pollution tolerance index (APTI) and anticipated performance index (API) for long-term air pollution abatement, most suitable plant species identified and recommended for development of urban forest in Varanasi, India, were Ficus benghalensis L. (APTI=26.01, API=6) and Ficus religiosa (APTI=23.35, API=6). Additional good performers were Polyalthia longifolia, Ficus glomerata (Roxb.), Anthocephalus indicus and Mangifera indica (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Pandey_2015” target=”_blank”&gt;Pandey et al., 2015&lt;/a&gt;). NO2 levels were found to be 7% lower in a forest stand than in nearby, non-canopy areas during all Fall sampling seasons (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grundstrom_2014” target=”_blank”&gt;Grundstrom and Pleijel, 2014&lt;/a&gt;). Urban streets with trees have been shown to have as much as 65% lower SO2 levels and lower suspended PM levels when compared to unbuffered streets (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Vailshery_2013” target=”_blank”&gt;Vailshery et al., 2013&lt;/a&gt;). Ozone uptake and removal was found to vary among tree type and season in Rome, with the highest removal in spring and summer by deciduous broadleaf species (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Manes_2012” target=”_blank”&gt;Manes et al., 2012&lt;/a&gt;). Tree stands consisting of multiple species removed greater amounts of O3 across annual differences in weather patterns, typical seasonal fluctuations, and variance in O3 concentrations than single tree species (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Manes_2014” target=”_blank”&gt;Manes et al., 2014). In northern climates with a short growing season, the ability of urban trees to remove air pollutants may be minimal (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Setala_2013” target=”_blank”&gt;Setala et al., 2013&lt;/a&gt;). However, another study found relatively comparable removal of NO2 and PM2.5 in summer and winter, with more removal in the winter (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#King_2014” target=”_blank”&gt;King et al., 2014&lt;/a&gt;). *Near-road vegetative buffers*  In addition to reducing ambient air pollution, trees and shrubbery can trap or divert vehicular air pollutants coming directly from a busy roadway (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Brantley_2014” target=”_blank”&gt;Brantley et al., 2014&lt;/a&gt;). Diesel exhaust and other harmful emissions are elevated beyond background levels as far as 500m from a road edge. Roadside greenbelts have been found to reduce total suspended particles by up to 65% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Islam_2012” target=”_blank”&gt;Islam et al., 2012&lt;/a&gt;). Higher greenness within and surrounding school boundaries (50m buffer) was associated with lower indoor and outdoor NO2, ultrafine particles, and traffic-related PM2.5 levels (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dadvand_2015” target=”_blank”&gt;Dadvand et al., 2015&lt;/a&gt;). The effectiveness of near-road vegetative buffers is highly dependent on local factors including temperature, precipitation wind speed and direction, design of the built environment, and human activity patterns (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wania_2012” target=”_blank”&gt;Wania et al., 2012&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mori_2015” target=”_blank”&gt;Mori et al., 2015&lt;/a&gt;). Particle concentrations may be higher directly underneath near-road tree canopy where it has become entrapped. Tall buildings in downtown areas can modify wind flow such that tree cover may exacerbate particle concentrations in urban &amp;quot;street canyons&amp;quot; (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wania_2012” target=”_blank”&gt;Wania et al., 2012&lt;/a&gt;). *Green roofs*  Modeling has shown that constructed green space--green roofs composed of grass or shrubs, and green walls supporting vines and other herbaceous plants--can augment the effect of ground-level trees and shrubs in air pollution mitigation (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Currie_2008” target=”_blank”&gt;Currie and Bass 2008&lt;/a&gt;). It has been estimated that 2000m&amp;#178; of uncut grass on a green roof can remove up to 4000 kg of particulate matter (Johnston and Newton, 1996). Green roofs also reduce air pollutants indirectly by decreasing building energy consumption and thus, emissions. *Urban parks*  Green space can reduce ambient urban air pollutant concentrations also by displacing pollutant sources, such as roads and buildings. Urban parks yielded mean values of 89ppb for NOx and 24 mG/m3 for PM10, while means for an urban street were 413ppb and 80 mG/m3, respectively. Dust mitigation was attributed to park trees, especially during dust flow episodes (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenP_2014” target=”_blank”&gt;Cohen et al., 2014&lt;/a&gt;). Vegetation can also increase air pollution through the production of pollen, fungal spores, and volatile organic compounds (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Prendez_2013” target=”_blank”&gt;Prendez et al., 2013), which contribute to ozone formation (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Calfapietra_2013” target=”_blank”&gt;Calfapietra et al., 2013&lt;/a&gt;).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urban ecosystems provide the opportunity to engage with nature through the use of urban green spaces such as parks, public and private gardens and urban forests. People who live close to green spaces may visit them more frequently (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Giles_2005” target=”_blank”&gt;Giles-Corti et al., 2005; Mowen et al., 2007&lt;/a&gt;). Positive correlations have been found between number of park visitors and number of trees and canopy coverage, as well as diversity of visitor activities (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Adinolfi_2014” target=”_blank”&gt;Adinolfi et al., 2014&lt;/a&gt;). Urban blue spaces have also been identified as popular places for leisure and recreational activities (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Volker_2013” target=”_blank”&gt;Volker &amp;amp; Kistemann 2013&lt;/a&gt;). Urban green and blue spaces, including public parks, private gardens, and promenades, provide areas for people to not only engage with nature, but to rest and interact (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Seeland_2009” target=”_blank”&gt;Seeland et al., 2009&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#WardCD_2010” target=”_blank”&gt;Ward et al., 2010&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Freeman_2012” target=”_blank”&gt;Freeman et al., 2012&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Volker_2013” target=”_blank”&gt;Volker &amp;amp; Kistemann 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#HanX_2013” target=”_blank”&gt;Han et al., 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Peschardt_2014” target=”_blank”&gt;Peschardt et al., 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Green spaces, along with even sporadic greenness such as street trees, increase local aesthetic value and are cooler than developed areas, encouraging people to spend more time outdoors. As plant species richness increased, visitors had a greater mean aesthetic appreciation of experimental grassland ecosystems (F4,95 = 71.1, p less than 0.001) and natural meadows (r = 0.75, F1,70 = 91.3, p less than 0.001) (Lindemann-Matthies et al., 2009&lt;/a&gt;). A study of Slovenic neighborhoods found that residents living in new developments that did not have many trees rated their communities less aesthetically appealing than those in older communities that had trees (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lestan_2014” target=”_blank”&gt;Lestan et al., 2014&lt;/a&gt;). Subjects who perceived the absence of greenery and other public assets (places to sit or walk, or safe places for children to play) in their neighborhoods were more likely to not have taken a walk of 1 mile or more in the last year (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Ellaway_2009” target=”_blank”&gt;Ellaway et al., 2009; n=1637, Scotland&lt;/a&gt;). A photo questionnaire assessing the relationship between two measures of street cover density (panoramic photographs and Google Earth aerial images) and landscape preference revealed that subjects preferred 41% and 20% tree cover, respectively (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jiang_2015” target=”_blank”&gt;Jiang et al., 2015&lt;/a&gt;). In a study of green roofs, interviewees reported more aesthetic benefit from green roofs when the vegetation was in their direct line of site (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Loder_2014” target=”_blank”&gt;Loder, 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Exercising, passively spending time in green environments, and even viewing them through a window, have been shown to have multiple positive effects on health (see the health linkages to Aesthetics &amp;amp; Engagement with Nature). Respondents in another study reported that green roofs provided stress reduction benefits and an overall calming effect when visible in an urban environment (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Loder_2014” target=”_blank”&gt;Loder, 2014&lt;/a&gt;). </t>
   </si>
   <si>
     <t>Missing Id: Lindemann-Matthies et al., 2009</t>
@@ -8139,9 +8123,6 @@
   </si>
   <si>
     <t xml:space="preserve">In arid urban landscapes, cooling islands are most often associated with trees and forests (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Shashua_2009” target=”_blank”&gt;Shashua-Bar et al., 2009&lt;/a&gt;). One study found that, for every 10% increase in vegetation cover by census block group, daytime mean temperature decreased by 2.8&amp;#176; C (5.04&amp;#176; F) in June and 2.4&amp;#176; C (4.32&amp;#176; F) in October (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Buyantuyev_2010” target=”_blank”&gt;Buyantuyev and Wu, 2010&lt;/a&gt;). Another study reported that vegetated cover (measured as normalized difference vegetation index) reduced ambient temperatures on low-humidity summer days by up to 25&amp;#176; C (45&amp;#176; F) compared to bare soil (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jenerette_2011” target=”_blank”&gt;Jenerette et al., 2011&lt;/a&gt;). Green residential areas had lower mean land surface temperature (21.7&amp;#176; C or 71.06&amp;#176; F) than public parks (22.3&amp;#176; C or 72.14&amp;#176; F) and industrial sites (24.4&amp;#176; C or 75.92&amp;#176; F), due to higher percent vegetative cover (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rotem_2015” target=”_blank”&gt;Rotem-Mindali et al., 2015&lt;/a&gt;). Drylands vegetation adapted to low-water conditions (xeric) was shown to have the greatest temperature reduction at night vs. daytime periods (e.g. -2.4 vs. -1 &amp;#176; C or 4.32 vs. -1.8&amp;#176; F) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Chow_2012” target=”_blank”&gt;Chow and Brazel, 2012&lt;/a&gt;). Green roofs were also shown to mitigate high temperatures in dryland urban areas. One study found that maximum green roof temperatures were 15-20&amp;#176; C (27-36&amp;#176; F) lower than those of bare rooftops (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nardini_2012” target=”_blank”&gt;Nardini et al., 2012&lt;/a&gt;). Another study found that succulent-based green roofs can provide significant rooftop temperature reductions of up to 27.5&amp;#176; C (49.5&amp;#176; F) during hot, dry summer conditions (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dvorak_2013” target=”_blank”&gt;Dvorak and Volder, 2013&lt;/a&gt;). &amp;#xD;&amp;#xD;During high temperature and humidity conditions in arid regions, thermal comfort is improved by the presence of vegetative cover. In areas with no vegetation, the Thermal Humidity Index (THI) in summertime was greater than 27&amp;#176; C or 80.6&amp;#176; F (the level where people begin to experience heat fatigue and other health risks). However, for vegetated areas including irrigated lawn, shade trees and a combination of both, THI was less than this threshold (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#SongJ_2015” target=”_blank”&gt;Song and Wang, 2015&lt;/a&gt;). When courtyards were shaded by trees or mesh, thermal stress was reduced by nearly a half and when combined with grass, it further produces a modest reduction in stress (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Shashua_2011” target=”_blank”&gt;Shashua-Bar et al., 2011&lt;/a&gt;). During the summer, human discomfort may be more pronounced in an urban vs. rural desert environment since irrigated urban green space (i.e. parks, lawns, and street trees) can increase air humidity and aggravate heat stress (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Potchter_2013” target=”_blank”&gt;Potchter and Ben-Shalom, 2013&lt;/a&gt;). Thermal discomfort (summarized by Thom&amp;#39;s discomfort index) can also be triggered when air pollution (PM10, NO2, and O3) is high during heat wave days (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Papanastasiou_2015” target=”_blank”&gt;Papanastasiou et al., 2015&lt;/a&gt;). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green spaces within urban areas can decrease daytime atmospheric temperatures through shading and evapotranspiration, thus decreasing the Urban Heat Island effect (UHI). Increasing vegetative cover and adding higher reflective surface materials in urban areas can reduce temperatures within the area (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jenerette_2011” target=”_blank”&gt;Jenerette et al., 2011; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rotem_2015” target=”_blank”&gt;Rotem-Mindali et al., 2015&lt;/a&gt;) and increase the amount of cooling energy savings; these benefits increase with time as trees mature and dead trees are replaced with new ones (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Solecki_2005” target=”_blank”&gt;Solecki et al., 2005&lt;/a&gt;). &amp;quot;Urban cooling islands&amp;quot; (UCIs) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Shashua_2009” target=”_blank”&gt;Shashua-Bar et al., 2009&lt;/a&gt;) are most often associated with urban trees and forests; one study linked a one-hectare increase in urban forest area to a mean temperature decrease of 0.5&amp;#176; Celsius (0.9&amp;#176; F) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kong_2014” target=”_blank”&gt;Kong et al., 2014&lt;/a&gt;). An urban drylands study found that, for every 10% increase in vegetation cover, daytime mean temperature in census block groups decreased by 2.8&amp;#176; C (5.04&amp;#176; F) in June and 2.4&amp;#176; C (4.32&amp;#176; F) in October (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Buyantuyev_2010” target=”_blank”&gt;Buyantuyev and Wu, 2010&lt;/a&gt;). Both grass and tree cover greatly affect surface and air temperatures: measures of grass temperature were up to 24&amp;#176; C (43.2&amp;#176; F) cooler than local maximum surface temperature (similar to model predictions), while temperatures in tree shade were up to 19&amp;#176; C (34.2&amp;#176; F) cooler (Armson, Stinger and Ennos 2012&lt;/a&gt;). High xeric vegetation cover adapted to low water availability was shown to have the greatest temperature reduction at night vs. daytime periods (e.g. -2.4 vs. -1 &amp;#176; C or 4.32 vs. -1.8&amp;#176; F) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Chow_2012” target=”_blank”&gt;Chow et al., 2012&lt;/a&gt;). &amp;#xD;&amp;#xD;The presence of shade trees can increase the daily average temperature at which air conditioning use begins, from 18.7 to 20.3&amp;#176; C (65.7&amp;#176; to 68.5&amp;#176; F), thus reducing summer energy usage (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Akbari_1997” target=”_blank”&gt;Akbari et al., 1997&lt;/a&gt;). In one study, street segments with trees had lower ambient temperatures by as much as 5.6&amp;#176; C (10.1&amp;#176; F) and lower surface temperatures by as much as 27.5&amp;#176; C (49.5 &amp;#176; F) when compared to exposed streets, indicating significant microclimatic buffering by trees (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Vailshery_2013” target=”_blank”&gt;Vailshery et al., 2013&lt;/a&gt;). Both the extent and configuration of green space are related to variability in urban temperatures. One study found that the most important influences on temperature were the shape and area of tree patches, and the connectivity of grass and shrub patches (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ChenA_2014” target=”_blank”&gt;Chen, 2014&lt;/a&gt;). Similarly, variables that combined percentage green space, edge density, and patch density explained the most variance in land surface temperature (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Maimaitiyiming_2014” target=”_blank”&gt;Maimaitiyiming et al., 2014&lt;/a&gt;). &amp;#xD;&amp;#xD; A study of green roofs found that maximum green roof temperatures were 15-20&amp;#176; C (27-36&amp;#176; F) lower than that of bare rooftops (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nardini_2012” target=”_blank”&gt;Nardini et al., 2012&lt;/a&gt;). A regional simulation model using 50% green-roof coveradge distributed evenly throughout a city showed ambient temperature reductions as great as 2&amp;#176; C (3.6&amp;#176; F) in some areas (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Bass_2003” target=”_blank”&gt;Bass et al., 2003&lt;/a&gt;). Another study found that succulent-based green roofs can provide rooftop temperature reductions of up to 27.5&amp;#176; C (49.5&amp;#176; F) during hot, dry summer conditions (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dvorak_2013” target=”_blank”&gt;Dvorak and Volder, 2013&lt;/a&gt;). &amp;#xD;&amp;#xD;In areas with no vegetation, the Thermal Humidity Index (THI) in summertime was greater than 27&amp;#176; C or 80.6&amp;#176; F (the level where people begin to experience heat fatigue and other health risks). However, for vegetated areas including irrigated lawn, shade trees and a combination of both, THI was less than this threshold (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#SongJ_2015” target=”_blank”&gt;Song and Wang, 2015&lt;/a&gt;). During the summer, human discomfort may be more pronounced in an urban vs. rural desert environment since irrigated urban green space (i.e. parks, lawns, and street trees) can increase air humidity and aggravate heat stress (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Potchter_2013” target=”_blank”&gt;Potchter and Ben-Shalom, 2013&lt;/a&gt;). Thermal discomfort (summarized by Thom&amp;#39;s discomfort index) can also be triggered when air pollution (PM10, NO2, and O3) is high during heat wave days (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Papanastasiou_2015” target=”_blank”&gt;Papanastasiou et al., 2015&lt;/a&gt;).  </t>
   </si>
   <si>
     <r>
@@ -8208,6 +8189,25 @@
   </si>
   <si>
     <t>Thomas_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Access or proximity to green space*  Many studies have found that people who live close to green space visit them more frequently and thus increase their time spent in physical activity, both at the green space itself and walking or biking to the area instead of driving (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Giles_2005” target=”_blank”&gt;Giles-Corti et al., 2005&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mowen_2007” target=”_blank”&gt;Mowen et al., 2007&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grigsby_2011” target=”_blank”&gt;Grigsby-Toussaint et al., 2011&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wendel_2004” target=”_blank”&gt;Wendel-Vos et al., 2004&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenDA_2006” target=”_blank”&gt;Cohen et al., 2006&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Edwards_2014” target=”_blank”&gt;Edwards et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#HanB_2014” target=”_blank”&gt;Han et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lachowycz_2014” target=”_blank”&gt;Lachowycz and Jones, 2014&lt;/a&gt;). One study found that living in an area with high parkland density (greater than 0.14%) increased the odds (OR=1.19) of meeting federal guidelines for MVPA and VPA (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#West_2012” target=”_blank”&gt;West et al., 2012&lt;/a&gt;). Another study found that as the density of public green space increased by one unit, walking was predicted to increase by 8.6% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Pliakas_2014” target=”_blank”&gt;Pliakas et al., 2014&lt;/a&gt;). A Swedish study found that people with green spaces within 50m of their homes visited those spaces 4x as much as those whose closest green space was 1km away (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grahn_2003” target=”_blank”&gt;Grahn and Stigsdotter, 2003&lt;/a&gt;). In San Diego, the presence of a park within a 50-meter buffer of each accelerometer study point was associated with 41% higher odds (OR 1.41) of light physical activity in adolescent females (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rodriguez_2012” target=”_blank”&gt;Rodriguez et al., 2012&lt;/a&gt;; n=293). However, several studies have found little to no association between access or proximity to green space and physical activity (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Hillsdon_2006” target=”_blank”&gt;Hillsdon et al., 2006&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Maas_2008” target=”_blank”&gt;Maas et al., 2008&lt;/a&gt;). *Amount and design of green space:* The size of nearby public open spaces has been positively associated with physical activity (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Paquet_2013” target=”_blank”&gt;Paquet et al., 2013&lt;/a&gt;; Fan et al., 2015&lt;/a&gt;). Positive correlations have been found between number of park visitors, as well as diversity of visitor activities, and number of trees and canopy coverage (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Adinolfi_2014” target=”_blank”&gt;Adinolfi et al., 2014&lt;/a&gt;). One study found that individuals living in the greenest urban quintile were 1.39 times more physically active than those living in the least green urban quintile (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mytton_2012” target=”_blank”&gt;Mytton et al., 2012&lt;/a&gt;). Another study reported that respondents whose residential environment contained high levels of greenery (on a scale from 1-5) were 3x more likely to be physically active, and 40% less likely to be overweight or obese (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Ellaway_2005” target=”_blank”&gt;Ellaway et al., 2005&lt;/a&gt;). Yet another study found that increased exposure to neighborhood greenness from 10th to 90th percentile was associated with a 34% to 39% increase in odds for moderate to vigorous physical activity (MVPA) in children (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Almanza_2012” target=”_blank”&gt;Almanza et al., 2012&lt;/a&gt;). Cross-sectional study of middle-school aged children found that a 5% increase in neighborhood area covered by trees was associated with 5% higher frequency of physical activity outside of school hours (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#JanssenI_2015” target=”_blank”&gt;Janssen and Rosu, 2015&lt;/a&gt;). Elderly men were shown to participate in regular physical activity when living within a 400-meter radius green space buffer around the home (OR=1.21) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Gong_2014” target=”_blank”&gt;Gong et al., 2014&lt;/a&gt;). Strong positive associations were reported between the odds of walking and both density of street trees and street network connectivity, and also between distance walked and both overall greenness and density of street trees (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Sarkar_2015” target=”_blank”&gt;Sarkar et al., 2015&lt;/a&gt;). &amp;#xD;&amp;#xD;In urban areas, street intersections and other pedestrian amenities are a promoting factor in physical activity (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wetter_2001” target=”_blank”&gt;Wetter et al., 2001&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kaczynski_2014” target=”_blank”&gt;Kaczynski et al., 2014&lt;/a&gt;). Children engaged in significantly greater amounts of MVPA and PA after the conversion of a traditional playground or school yard into one modeled on natural environments (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Coe_2014” target=”_blank”&gt;Coe et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#JanssonM_2014” target=”_blank”&gt;Jansson et al., 2014&lt;/a&gt;), or when community spaces were comprised of vegetation, open meadows, and/or undulating topography (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lestan_2014” target=”_blank”&gt;Lestan et al., 2014&lt;/a&gt;). However, while school areas with the greatest amount of green space were among children&amp;#39;s favorites, the areas of mixed green and built environments were where the most physical activity took place (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Martensson_2014” target=”_blank”&gt;Martensson et al., 2014&lt;/a&gt;). *Perceptions of green space* Increases in individual satisfaction with neighborhood green space, perception of recreation areas, and perception of their easy access were found to be contributing factors to increases in overall MVPA and PA in parks (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Bai_2013” target=”_blank”&gt;
+Bai et al., 2013&lt;/a&gt;; Jeppesen et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jongeneel_2014” target=”_blank”&gt;Jongeneel-Grimen et al., 2014&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#LeeJ_2014” target=”_blank”&gt;Lee et al., 2014&lt;/a&gt;). A multi-country study found that adult recreational walking was strongly associated with perceived neighborhood environmental attributes such as land use mix, street connectivity and aesthetics (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Sugiyama_2014” target=”_blank”&gt;Sugiyama et al., 2014&lt;/a&gt;). One study found that, in a living environment perceived as green, 62% of the aging population engaged in high levels of physical activity while only 11% engaged in physical activity in an environment perceived as containing little green space (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kemperman_2014” target=”_blank”&gt;Kemperman and Timmermans, 2014&lt;/a&gt;). Also, being nature-oriented was more important than park access as a predictor of park use (p less than 0.01) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lin_2014” target=”_blank”&gt;Lin et al., 2014&lt;/a&gt;). &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZhangW_2015” target=”_blank”&gt;Zhang et al. (2015)&lt;/a&gt; found that five variables had significant effects on respondents&amp;#39; satisfaction levels when participating in physical activities in urban green spaces: housing price of the residential units where respondents lived (p=0.001), travel time to the nearest park (p less than 0.0001), counts of types of green spaces available for physical activities (p=0.04), and the rating of vegetation (p less than 0.0001). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban ecosystems provide the opportunity to engage with nature through the use of urban green spaces such as parks, public and private gardens and urban forests. People who live close to green spaces may visit them more frequently (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Giles_2005” target=”_blank”&gt;Giles-Corti et al., 2005&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mowen_2007” target=”_blank”&gt;Mowen et al., 2007&lt;/a&gt;). Positive correlations have been found between number of park visitors and number of trees and canopy coverage, as well as diversity of visitor activities (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Adinolfi_2014” target=”_blank”&gt;Adinolfi et al., 2014&lt;/a&gt;). Urban blue spaces have also been identified as popular places for leisure and recreational activities (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Volker_2013” target=”_blank”&gt;Volker &amp;amp; Kistemann 2013&lt;/a&gt;). Urban green and blue spaces, including public parks, private gardens, and promenades, provide areas for people to not only engage with nature, but to rest and interact (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Seeland_2009” target=”_blank”&gt;Seeland et al., 2009&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#WardCD_2010” target=”_blank”&gt;Ward et al., 2010&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Freeman_2012” target=”_blank”&gt;Freeman et al., 2012&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Volker_2013” target=”_blank”&gt;Volker &amp;amp; Kistemann 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#HanX_2013” target=”_blank”&gt;Han et al., 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Peschardt_2014” target=”_blank”&gt;Peschardt et al., 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Green spaces, along with even sporadic greenness such as street trees, increase local aesthetic value and are cooler than developed areas, encouraging people to spend more time outdoors. As plant species richness increased, visitors had a greater mean aesthetic appreciation of experimental grassland ecosystems (F4,95 = 71.1, p less than 0.001) and natural meadows (r = 0.75, F1,70 = 91.3, p less than 0.001) (Lindemann-Matthies et al., 2009&lt;/a&gt;). A study of Slovenic neighborhoods found that residents living in new developments that did not have many trees rated their communities less aesthetically appealing than those in older communities that had trees (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Lestan_2014” target=”_blank”&gt;Lestan et al., 2014&lt;/a&gt;). Subjects who perceived the absence of greenery and other public assets (places to sit or walk, or safe places for children to play) in their neighborhoods were more likely to not have taken a walk of 1 mile or more in the last year (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Ellaway_2009” target=”_blank”&gt;Ellaway et al., 2009&lt;/a&gt;; n=1637, Scotland). A photo questionnaire assessing the relationship between two measures of street cover density (panoramic photographs and Google Earth aerial images) and landscape preference revealed that subjects preferred 41% and 20% tree cover, respectively (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jiang_2015” target=”_blank”&gt;Jiang et al., 2015&lt;/a&gt;). In a study of green roofs, interviewees reported more aesthetic benefit from green roofs when the vegetation was in their direct line of site (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Loder_2014” target=”_blank”&gt;Loder, 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Exercising, passively spending time in green environments, and even viewing them through a window, have been shown to have multiple positive effects on health (see the health linkages to Aesthetics &amp;amp; Engagement with Nature). Respondents in another study reported that green roofs provided stress reduction benefits and an overall calming effect when visible in an urban environment (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Loder_2014” target=”_blank”&gt;Loder, 2014&lt;/a&gt;). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green spaces within urban areas can decrease daytime atmospheric temperatures through shading and evapotranspiration, thus decreasing the Urban Heat Island effect (UHI). Increasing vegetative cover and adding higher reflective surface materials in urban areas can reduce temperatures within the area (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Jenerette_2011” target=”_blank”&gt;Jenerette et al., 2011&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rotem_2015” target=”_blank”&gt;Rotem-Mindali et al., 2015&lt;/a&gt;) and increase the amount of cooling energy savings; these benefits increase with time as trees mature and dead trees are replaced with new ones (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Solecki_2005” target=”_blank”&gt;Solecki et al., 2005&lt;/a&gt;). &amp;quot;Urban cooling islands&amp;quot; (UCIs) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Shashua_2009” target=”_blank”&gt;Shashua-Bar et al., 2009&lt;/a&gt;) are most often associated with urban trees and forests; one study linked a one-hectare increase in urban forest area to a mean temperature decrease of 0.5&amp;#176; Celsius (0.9&amp;#176; F) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Kong_2014” target=”_blank”&gt;Kong et al., 2014&lt;/a&gt;). An urban drylands study found that, for every 10% increase in vegetation cover, daytime mean temperature in census block groups decreased by 2.8&amp;#176; C (5.04&amp;#176; F) in June and 2.4&amp;#176; C (4.32&amp;#176; F) in October (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Buyantuyev_2010” target=”_blank”&gt;Buyantuyev and Wu, 2010&lt;/a&gt;). Both grass and tree cover greatly affect surface and air temperatures: measures of grass temperature were up to 24&amp;#176; C (43.2&amp;#176; F) cooler than local maximum surface temperature (similar to model predictions), while temperatures in tree shade were up to 19&amp;#176; C (34.2&amp;#176; F) cooler (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Armson_2012” target=”_blank”&gt;Armson, Stinger and Ennos 2012&lt;/a&gt;). High xeric vegetation cover adapted to low water availability was shown to have the greatest temperature reduction at night vs. daytime periods (e.g. -2.4 vs. -1 &amp;#176; C or 4.32 vs. -1.8&amp;#176; F) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Chow_2012” target=”_blank”&gt;Chow et al., 2012&lt;/a&gt;). &amp;#xD;&amp;#xD;The presence of shade trees can increase the daily average temperature at which air conditioning use begins, from 18.7 to 20.3&amp;#176; C (65.7&amp;#176; to 68.5&amp;#176; F), thus reducing summer energy usage (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Akbari_1997” target=”_blank”&gt;Akbari et al., 1997&lt;/a&gt;). In one study, street segments with trees had lower ambient temperatures by as much as 5.6&amp;#176; C (10.1&amp;#176; F) and lower surface temperatures by as much as 27.5&amp;#176; C (49.5 &amp;#176; F) when compared to exposed streets, indicating significant microclimatic buffering by trees (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Vailshery_2013” target=”_blank”&gt;Vailshery et al., 2013&lt;/a&gt;). Both the extent and configuration of green space are related to variability in urban temperatures. One study found that the most important influences on temperature were the shape and area of tree patches, and the connectivity of grass and shrub patches (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ChenA_2014” target=”_blank”&gt;Chen, 2014&lt;/a&gt;). Similarly, variables that combined percentage green space, edge density, and patch density explained the most variance in land surface temperature (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Maimaitiyiming_2014” target=”_blank”&gt;Maimaitiyiming et al., 2014&lt;/a&gt;). &amp;#xD;&amp;#xD; A study of green roofs found that maximum green roof temperatures were 15-20&amp;#176; C (27-36&amp;#176; F) lower than that of bare rooftops (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nardini_2012” target=”_blank”&gt;Nardini et al., 2012&lt;/a&gt;). A regional simulation model using 50% green-roof coveradge distributed evenly throughout a city showed ambient temperature reductions as great as 2&amp;#176; C (3.6&amp;#176; F) in some areas (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Bass_2003” target=”_blank”&gt;Bass et al., 2003&lt;/a&gt;). Another study found that succulent-based green roofs can provide rooftop temperature reductions of up to 27.5&amp;#176; C (49.5&amp;#176; F) during hot, dry summer conditions (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dvorak_2013” target=”_blank”&gt;Dvorak and Volder, 2013&lt;/a&gt;). &amp;#xD;&amp;#xD;In areas with no vegetation, the Thermal Humidity Index (THI) in summertime was greater than 27&amp;#176; C or 80.6&amp;#176; F (the level where people begin to experience heat fatigue and other health risks). However, for vegetated areas including irrigated lawn, shade trees and a combination of both, THI was less than this threshold (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#SongJ_2015” target=”_blank”&gt;Song and Wang, 2015&lt;/a&gt;). During the summer, human discomfort may be more pronounced in an urban vs. rural desert environment since irrigated urban green space (i.e. parks, lawns, and street trees) can increase air humidity and aggravate heat stress (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Potchter_2013” target=”_blank”&gt;Potchter and Ben-Shalom, 2013&lt;/a&gt;). Thermal discomfort (summarized by Thom&amp;#39;s discomfort index) can also be triggered when air pollution (PM10, NO2, and O3) is high during heat wave days (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Papanastasiou_2015” target=”_blank”&gt;Papanastasiou et al., 2015&lt;/a&gt;).  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various ecologically-based filtration systems, constructed in locations where urban stormwater runs or accumulates, have been shown to reduce contaminants in water by 29 to 99% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Birch_2005” target=”_blank”&gt;Birch et al., 2005&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#DiBlasi_2008” target=”_blank”&gt;DiBlasi et al., 2008&lt;/a&gt;). These systems can include stormwater infiltration basins, grass swales, rain gardens, and stormwater bioretention facilities. The systems were able to remove 69% of suspended solids, 46% of phosphorous (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Deletic_2006” target=”_blank”&gt;Deletic and Fletcher, 2006&lt;/a&gt;), 51-56% of nitrogen (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dietz_2005” target=”_blank”&gt;Dietz and Clausen, 2005&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Deletic_2006” target=”_blank”&gt;Deletic and Fletcher, 2006&lt;/a&gt;), 90% of polycyclic aromatic hydrocarbons (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#DiBlasi_2008” target=”_blank”&gt;DiBlasi et al., 2008&lt;/a&gt;), and 29-93% of heavy metals (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Birch_2005” target=”_blank”&gt;Birch et al., 2005&lt;/a&gt;). A large nursery-based study evaluated the effectiveness of 9 native plants in their nutrient (PO4-3, NH3, NO3-) removal capacity from urban stormwater. Six of the best performers (Agapanthus, Pennisetum, Stenotaphrum, Zantedeschia, Phragmites and Typha) removed 16% more PO4-3 compared to soil-only control; two plant types (Pennisetum and Stenotaphrum) were 22% more effective in removing NH3 compared to control, and five (Agapanthus, Carpobrotus, Ficinia, Zantedeschia and Typha) removed 27-53% more NO3- compared to their controls (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Milandri_2012” target=”_blank”&gt;Milandri et al., 2012&lt;/a&gt;). </t>
+  </si>
+  <si>
+    <t>Urban tree cover and other green space can reduce local concentrations of harmful air pollutants. *Mitigation of PM10*  Multiple modeling studies have linked tree cover to a 1-2% local reduction in particulate matter smaller than 10 micrometers (PM10). Annually, this can equate to more than 100 metric tons in Mexico City (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Baumgardner_2012” target=”_blank”&gt;Baumgardner et al., 2012&lt;/a&gt;) and more than 2,000 metric tons in the city of London (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Tallis_2011” target=”_blank”&gt;Tallis et al., 2011&lt;/a&gt;). With strategic tree placement, annual reductions in ambient concentrations of PM10 may reach 7-20% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Bealey_2006” target=”_blank”&gt;Bealey et al., 2006&lt;/a&gt;). Hedge shrubbery has been found to collect PM10 with 34% efficiency (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Tiwary_2008” target=”_blank”&gt;Tiwary et al., 2008&lt;/a&gt;). Conifers and broad-leaved species with rough surfaces, and species with high leaf wax capture the highest quantities of PM (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Beckett_2000” target=”_blank”&gt;Beckett et al., 2000&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Popek_2013” target=”_blank”&gt;Popek et al., 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Rasanen_2013” target=”_blank”&gt;Rasanen et al., 2013&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nguyen_2015” target=”_blank”&gt;Nguyen et al., 2015&lt;/a&gt;). *Urban tree cover and mitigation of additional air pollutants*  In addition to PM10, trees can reduce ambient concentrations of PM2.5, ultrafine particles (less than 1 micrometer) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Beckett_2000” target=”_blank”&gt;Beckett et al., 2000&lt;/a&gt;) and gaseous pollutants including ozone, nitrogen dioxide, sulfur dioxide, and carbon monoxide (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Nowak_1994” target=”_blank”&gt;Nowak et al., 1994&lt;/a&gt;). Based on an air pollution tolerance index (APTI) and anticipated performance index (API) for long-term air pollution abatement, most suitable plant species identified and recommended for development of urban forest in Varanasi, India, were Ficus benghalensis L. (APTI=26.01, API=6) and Ficus religiosa (APTI=23.35, API=6). Additional good performers were Polyalthia longifolia, Ficus glomerata (Roxb.), Anthocephalus indicus and Mangifera indica (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Pandey_2015” target=”_blank”&gt;Pandey et al., 2015&lt;/a&gt;). NO2 levels were found to be 7% lower in a forest stand than in nearby, non-canopy areas during all Fall sampling seasons (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grundstrom_2014” target=”_blank”&gt;Grundstrom and Pleijel, 2014&lt;/a&gt;). Urban streets with trees have been shown to have as much as 65% lower SO2 levels and lower suspended PM levels when compared to unbuffered streets (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Vailshery_2013” target=”_blank”&gt;Vailshery et al., 2013&lt;/a&gt;). Ozone uptake and removal was found to vary among tree type and season in Rome, with the highest removal in spring and summer by deciduous broadleaf species (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Manes_2012” target=”_blank”&gt;Manes et al., 2012&lt;/a&gt;). Tree stands consisting of multiple species removed greater amounts of O3 across annual differences in weather patterns, typical seasonal fluctuations, and variance in O3 concentrations than single tree species (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Manes_2014” target=”_blank”&gt;Manes et al., 2014)&lt;/a&gt;. In northern climates with a short growing season, the ability of urban trees to remove air pollutants may be minimal (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Setala_2013” target=”_blank”&gt;Setala et al., 2013&lt;/a&gt;). However, another study found relatively comparable removal of NO2 and PM2.5 in summer and winter, with more removal in the winter (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#King_2014” target=”_blank”&gt;King et al., 2014&lt;/a&gt;). *Near-road vegetative buffers*  In addition to reducing ambient air pollution, trees and shrubbery can trap or divert vehicular air pollutants coming directly from a busy roadway (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Brantley_2014” target=”_blank”&gt;Brantley et al., 2014&lt;/a&gt;). Diesel exhaust and other harmful emissions are elevated beyond background levels as far as 500m from a road edge. Roadside greenbelts have been found to reduce total suspended particles by up to 65% (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Islam_2012” target=”_blank”&gt;Islam et al., 2012&lt;/a&gt;). Higher greenness within and surrounding school boundaries (50m buffer) was associated with lower indoor and outdoor NO2, ultrafine particles, and traffic-related PM2.5 levels (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dadvand_2015” target=”_blank”&gt;Dadvand et al., 2015&lt;/a&gt;). The effectiveness of near-road vegetative buffers is highly dependent on local factors including temperature, precipitation wind speed and direction, design of the built environment, and human activity patterns (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wania_2012” target=”_blank”&gt;Wania et al., 2012&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Mori_2015” target=”_blank”&gt;Mori et al., 2015&lt;/a&gt;). Particle concentrations may be higher directly underneath near-road tree canopy where it has become entrapped. Tall buildings in downtown areas can modify wind flow such that tree cover may exacerbate particle concentrations in urban &amp;quot;street canyons&amp;quot; (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Wania_2012” target=”_blank”&gt;Wania et al., 2012&lt;/a&gt;). *Green roofs*  Modeling has shown that constructed green space--green roofs composed of grass or shrubs, and green walls supporting vines and other herbaceous plants--can augment the effect of ground-level trees and shrubs in air pollution mitigation (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Currie_2008” target=”_blank”&gt;Currie and Bass 2008&lt;/a&gt;). It has been estimated that 2000m&amp;#178; of uncut grass on a green roof can remove up to 4000 kg of particulate matter (Johnston and Newton, 1996). Green roofs also reduce air pollutants indirectly by decreasing building energy consumption and thus, emissions. *Urban parks*  Green space can reduce ambient urban air pollutant concentrations also by displacing pollutant sources, such as roads and buildings. Urban parks yielded mean values of 89ppb for NOx and 24 mG/m3 for PM10, while means for an urban street were 413ppb and 80 mG/m3, respectively. Dust mitigation was attributed to park trees, especially during dust flow episodes (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenP_2014” target=”_blank”&gt;Cohen et al., 2014&lt;/a&gt;). Vegetation can also increase air pollution through the production of pollen, fungal spores, and volatile organic compounds (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Prendez_2013” target=”_blank”&gt;Prendez et al., 2013&lt;/a&gt;), which contribute to ozone formation (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Calfapietra_2013” target=”_blank”&gt;Calfapietra et al., 2013&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetative cover in urban and rural desert environments can reduce ambient air pollutant concentrations both by removal and by airflow displacement. Pinyon-juniper stands have shown the highest capacity to remove criteria air pollutants (e.g., PM10, O3, NO2), followed by shrublands and grasslands (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Dicus_2009” target=”_blank”&gt;Dicus et al., 2009&lt;/a&gt;). Mean ambient NOx and PM10 have been measured at 89ppb and 24 mg/m3, respectively, in urban parks, while means for an urban street were 413ppb and 80 mg/m3, respectively (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenP_2014” target=”_blank”&gt;Cohen et al., 2014&lt;/a&gt;). &amp;#xD;&amp;#xD;Dust storms are frequent in dryland environments, where low-pressure and high wind-speed conditions can increase average PM2.5 and PM10 concentrations (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#ZangR_2008” target=”_blank”&gt;Zhang et al., 2008&lt;/a&gt;; &lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Hosseini_2015” target=”_blank”&gt;Hosseini et al., 2015&lt;/a&gt;). Naturally-occurring biological soil crusts (biocrusts) and vegetative cover (e.g., trees, shrubs, grasses) can decrease soil erosion rates by holding soil in place and/or by reducing wind. For example, during periods of dust flow, park trees were found to reduce PM10 from 218 micro-g/m3 to 64 micro-g/m3 (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#CohenP_2014” target=”_blank”&gt;Cohen et al., 2014&lt;/a&gt;). Significant negative correlation (-0.59 at 99% CI) have been observed between vegetative cover and occurrences of spring dust storms (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Zou_2004” target=”_blank”&gt;Zou and Zhai 2004&lt;/a&gt;). Experimental plots with 100% grass cover reductions experienced 10 times greater erosion rates than control plots with 0% grass cover reductions (p=0.05) (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#LiJ_2007” target=”_blank”&gt;Li et al., 2007&lt;/a&gt;). Furrowing and seeding three native perennial shrubs and bunch grass in previously tilled or over-grazed land helped reduce fugitive dust emissions by more than 80% by adequately stabilizing soil (&lt;a href=”https://enviroatlas.epa.gov/enviroatlas/Tools/EcoHealth_RelationshipBrowser/bibliography.html#Grants_1998” target=”_blank”&gt;Grantz et al., 1998)&lt;/a&gt;. At wind velocities of 18, 22, and 25 m/s, soil covered with 90% biocrust had wind erosion rates (g/min) 46, 21, and 17 times lower than those on sandy soil with 0% biocrust (Zhang et al., 2006). </t>
   </si>
 </sst>
 </file>
@@ -8898,8 +8898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8942,7 +8942,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2600</v>
+        <v>2680</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>260</v>
@@ -8960,13 +8960,13 @@
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>261</v>
       </c>
       <c r="F3" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="237" customHeight="1" x14ac:dyDescent="0.25">
@@ -8981,13 +8981,13 @@
         <v>28</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>2604</v>
+        <v>2677</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>262</v>
       </c>
       <c r="F4" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
@@ -9002,16 +9002,16 @@
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2678</v>
+        <v>2679</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>263</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>2679</v>
+        <v>2673</v>
       </c>
       <c r="G5" t="s">
-        <v>2676</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
@@ -9026,7 +9026,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>2625</v>
+        <v>2681</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>264</v>
@@ -9044,13 +9044,13 @@
         <v>361</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>2626</v>
+        <v>2678</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>265</v>
       </c>
       <c r="F7" t="s">
-        <v>2627</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="285" x14ac:dyDescent="0.25">
@@ -9065,13 +9065,13 @@
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>266</v>
       </c>
       <c r="F8" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -9086,7 +9086,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>267</v>
@@ -9104,13 +9104,13 @@
         <v>361</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>268</v>
       </c>
       <c r="F10" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="360" x14ac:dyDescent="0.25">
@@ -9125,7 +9125,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2628</v>
+        <v>2623</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>269</v>
@@ -9143,7 +9143,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2629</v>
+        <v>2624</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>270</v>
@@ -9161,7 +9161,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>2624</v>
+        <v>2621</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>271</v>
@@ -9179,7 +9179,7 @@
         <v>361</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>272</v>
@@ -9197,7 +9197,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>273</v>
@@ -9215,13 +9215,13 @@
         <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2622</v>
+        <v>2682</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>274</v>
       </c>
       <c r="F16" t="s">
-        <v>2623</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="210" x14ac:dyDescent="0.25">
@@ -9236,7 +9236,7 @@
         <v>361</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>275</v>
@@ -9254,13 +9254,13 @@
         <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2677</v>
+        <v>2672</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2680</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -9275,13 +9275,13 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>277</v>
       </c>
       <c r="F19" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="255" x14ac:dyDescent="0.25">
@@ -9296,7 +9296,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>278</v>
@@ -9314,7 +9314,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>279</v>
@@ -9332,13 +9332,13 @@
         <v>24</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>280</v>
       </c>
       <c r="F22" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -9359,7 +9359,7 @@
         <v>281</v>
       </c>
       <c r="F23" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="210" x14ac:dyDescent="0.25">
@@ -9374,13 +9374,13 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>282</v>
       </c>
       <c r="F24" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
   </sheetData>
@@ -9393,7 +9393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -10776,7 +10776,7 @@
         <v>295</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>2635</v>
+        <v>2630</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -10851,7 +10851,7 @@
         <v>298</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>2633</v>
+        <v>2628</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
@@ -11206,7 +11206,7 @@
         <v>313</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>2634</v>
+        <v>2629</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
@@ -11291,7 +11291,7 @@
         <v>316</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>2632</v>
+        <v>2627</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
@@ -11316,7 +11316,7 @@
         <v>317</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>2631</v>
+        <v>2626</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
@@ -11561,7 +11561,7 @@
         <v>327</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>2630</v>
+        <v>2625</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
@@ -11690,7 +11690,7 @@
         <v>331</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>2637</v>
+        <v>2632</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
@@ -11875,14 +11875,14 @@
         <v>339</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>2641</v>
+        <v>2636</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F97" si="2">IF(ISBLANK(SEARCH("&lt;/p&gt;&lt;p&gt;",E67)),1,0)</f>
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>2640</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -11900,7 +11900,7 @@
         <v>340</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>2639</v>
+        <v>2634</v>
       </c>
       <c r="F68">
         <f t="shared" si="2"/>
@@ -11922,7 +11922,7 @@
         <v>341</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>2642</v>
+        <v>2637</v>
       </c>
       <c r="F69">
         <f t="shared" si="2"/>
@@ -11944,7 +11944,7 @@
         <v>342</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>2643</v>
+        <v>2638</v>
       </c>
       <c r="F70">
         <f t="shared" si="2"/>
@@ -11966,7 +11966,7 @@
         <v>343</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>2638</v>
+        <v>2633</v>
       </c>
       <c r="F71">
         <f t="shared" si="2"/>
@@ -11988,7 +11988,7 @@
         <v>344</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>2636</v>
+        <v>2631</v>
       </c>
       <c r="F72">
         <f t="shared" si="2"/>
@@ -12010,7 +12010,7 @@
         <v>313</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>2672</v>
+        <v>2667</v>
       </c>
       <c r="F73">
         <f t="shared" si="2"/>
@@ -12032,14 +12032,14 @@
         <v>345</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>2674</v>
+        <v>2669</v>
       </c>
       <c r="F74">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>2673</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
@@ -12057,7 +12057,7 @@
         <v>346</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>2645</v>
+        <v>2640</v>
       </c>
       <c r="F75">
         <f t="shared" si="2"/>
@@ -12079,7 +12079,7 @@
         <v>347</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>2646</v>
+        <v>2641</v>
       </c>
       <c r="F76">
         <f t="shared" si="2"/>
@@ -12101,14 +12101,14 @@
         <v>348</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>2670</v>
+        <v>2665</v>
       </c>
       <c r="F77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>2671</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -12126,7 +12126,7 @@
         <v>349</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>2644</v>
+        <v>2639</v>
       </c>
       <c r="F78">
         <f t="shared" si="2"/>
@@ -12151,14 +12151,14 @@
         <v>350</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>2668</v>
+        <v>2663</v>
       </c>
       <c r="F79">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>2669</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -12176,7 +12176,7 @@
         <v>351</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>2647</v>
+        <v>2642</v>
       </c>
       <c r="F80">
         <f t="shared" si="2"/>
@@ -12195,7 +12195,7 @@
         <v>30</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>2658</v>
+        <v>2653</v>
       </c>
       <c r="F81">
         <f t="shared" si="2"/>
@@ -12214,7 +12214,7 @@
         <v>30</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>2657</v>
+        <v>2652</v>
       </c>
       <c r="F82">
         <f t="shared" si="2"/>
@@ -12236,13 +12236,13 @@
         <v>352</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>2665</v>
+        <v>2660</v>
       </c>
       <c r="F83" t="s">
-        <v>2666</v>
+        <v>2661</v>
       </c>
       <c r="G83" t="s">
-        <v>2667</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -12260,14 +12260,14 @@
         <v>353</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>2663</v>
+        <v>2658</v>
       </c>
       <c r="F84">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>2664</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -12285,7 +12285,7 @@
         <v>354</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>2675</v>
+        <v>2670</v>
       </c>
       <c r="F85">
         <f t="shared" si="2"/>
@@ -12304,7 +12304,7 @@
         <v>30</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>2656</v>
+        <v>2651</v>
       </c>
       <c r="F86">
         <f t="shared" si="2"/>
@@ -12323,7 +12323,7 @@
         <v>30</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>2655</v>
+        <v>2650</v>
       </c>
       <c r="F87">
         <f t="shared" si="2"/>
@@ -12345,14 +12345,14 @@
         <v>355</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>2661</v>
+        <v>2656</v>
       </c>
       <c r="F88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>2662</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>24</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>2654</v>
+        <v>2649</v>
       </c>
       <c r="F89">
         <f t="shared" si="2"/>
@@ -12389,7 +12389,7 @@
         <v>356</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>2660</v>
+        <v>2655</v>
       </c>
       <c r="F90">
         <f t="shared" si="2"/>
@@ -12408,7 +12408,7 @@
         <v>24</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>2653</v>
+        <v>2648</v>
       </c>
       <c r="F91">
         <f t="shared" si="2"/>
@@ -12430,7 +12430,7 @@
         <v>357</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>2659</v>
+        <v>2654</v>
       </c>
       <c r="F92">
         <f t="shared" si="2"/>
@@ -12449,7 +12449,7 @@
         <v>24</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>2652</v>
+        <v>2647</v>
       </c>
       <c r="F93">
         <f t="shared" si="2"/>
@@ -12468,7 +12468,7 @@
         <v>24</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>2651</v>
+        <v>2646</v>
       </c>
       <c r="F94">
         <f t="shared" si="2"/>
@@ -12487,7 +12487,7 @@
         <v>24</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>2650</v>
+        <v>2645</v>
       </c>
       <c r="F95">
         <f t="shared" si="2"/>
@@ -12506,7 +12506,7 @@
         <v>24</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>2649</v>
+        <v>2644</v>
       </c>
       <c r="F96">
         <f t="shared" si="2"/>
@@ -12525,7 +12525,7 @@
         <v>24</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>2648</v>
+        <v>2643</v>
       </c>
       <c r="F97">
         <f t="shared" si="2"/>
@@ -12543,9 +12543,9 @@
   <dimension ref="A1:H735"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A627" sqref="A627"/>
+      <selection pane="bottomLeft" activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19456,13 +19456,13 @@
     </row>
     <row r="627" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A627" s="6" t="s">
-        <v>2681</v>
+        <v>2675</v>
       </c>
       <c r="B627" s="6" t="s">
         <v>1697</v>
       </c>
       <c r="C627" s="7" t="s">
-        <v>2682</v>
+        <v>2676</v>
       </c>
       <c r="H627" s="1"/>
     </row>

</xml_diff>